<commit_message>
Added sparklines with reactable
</commit_message>
<xml_diff>
--- a/data/cranberry_recipes.xlsx
+++ b/data/cranberry_recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\RLadiesBoston\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53133A4-65FD-4550-A7CC-1AD0CDDBED51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41484AF9-4D63-4ABF-85C0-57C3D696FC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2190" windowWidth="19320" windowHeight="13365" xr2:uid="{5D967B9B-315C-4C32-B106-D2F44D14B1C1}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>Ingredients</t>
   </si>
   <si>
-    <t>2 cups peeled chopped apple, 3/4 cup sugar, 2 tablespoons oil, 1 egg, 1 1/2 cups flour. 1 1/2 teaspoons baking powder, 1/2 teaspoon baking soda, 1 teaspoon cinnamon, 1 cup cranberries (fresh or frozen), 1/2 cup chopped walnuts</t>
-  </si>
-  <si>
     <t>Instructions</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Cranberry Nut Bread</t>
   </si>
   <si>
-    <t>2 cups flour, 1 cup sugar, 1 1/2 teaspoons baking powder, 1 teaspoon salt, 1/2 teaspoon baking soda, 3/4 cup orange juice, 1 tablespoon grated orange peel, 2 tablespoons shortening, 1 egg, well beaten, 1 1/2 cups coarsely chopped fresh or frozen cranberries, 1/2 cup chopped nuts</t>
-  </si>
-  <si>
     <t>Harvest Apple Cranberry Cake</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
   </si>
   <si>
     <t>King Arthur Flour</t>
-  </si>
-  <si>
-    <t>1 tablespoon (14g) butter, melted, 1 tablespoon (21g) boiled cider, optional, 1 1/2 cups (170g) fresh or frozen whole cranberries, 1 cup (113g) peeled diced fresh apple (about 1 medium-large apple), 1/4 cup (50g) sugar, 1 1/2 cups (180g) Unbleached All-Purpose Flour, heaping 1/2 teaspoon salt, 1 1/2 teaspoons baking powder, 1 teaspoon ground cinnamon, 2/3 cup (131g) sugar, 2/3 cup (170g) applesauce, unsweetened preferred, 8 tablespoons (113g) butter, melted, 2 large eggs, 1 teaspoon vanilla extract</t>
   </si>
   <si>
     <t>Preheat oven to 350F. Grease an 8 1/2 x 4 1/2 x 2 1/2-inch loaf pan. Combine apples, sugar and oil in a medium mixing bowl. Add egg, mixing well. Combine dry ingredients in a separate mixing bowl. Add to apple mixture, mixing just until the dry ingredients are moist. Stir in cranberries and walnuts. Spread batter evenly in loaf pan. Bake for 1 hour or until a toothpick inserted into the center of the bread comes out clean. Makes 1 loaf.</t>
@@ -91,6 +82,15 @@
   </si>
   <si>
     <t>OriginalSource</t>
+  </si>
+  <si>
+    <t>2C peeled chopped apple, 3/4C sugar, 2T oil, 1 egg, 1 1/2C flour. 1 1/2t  baking powder, 1/2t baking soda, 1t cinnamon, 1C cranberries, 1/2C chopped walnuts</t>
+  </si>
+  <si>
+    <t>2C flour, 1C sugar, 1 1/2t baking powder, 1t salt, 1/2t baking soda, 3/4C orange juice, 1T grated orange peel, 2T shortening, 1 egg, well beaten, 1 1/2C coarsely chopped cranberries, 1/2C chopped nuts</t>
+  </si>
+  <si>
+    <t>1T butter-melted, 1T boiled cider, optional, 1 1/2C whole cranberries, 1C peeled diced fresh apple, 1/4C sugar, 1 1/2C Unbleached All-Purpose Flour, heaping 1/2t salt, 1 1/2t baking powder, 1t ground cinnamon, 2/3C sugar, 2/3C applesauce (unsweetened preferred), 8Tbutter-melted, 2 large eggs, 1t vanilla extract</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,13 +476,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,50 +490,50 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>